<commit_message>
Results of EH team today, Bug 5810 - Multi Assembly_joint
</commit_message>
<xml_diff>
--- a/etc/ap242/EH_XML_Examples/OccurencesNb.xlsx
+++ b/etc/ap242/EH_XML_Examples/OccurencesNb.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="175">
   <si>
     <t>Occurrence</t>
   </si>
@@ -36,18 +36,12 @@
     <t>_201007</t>
   </si>
   <si>
-    <t>_201008</t>
-  </si>
-  <si>
     <t>end a</t>
   </si>
   <si>
     <t>end b</t>
   </si>
   <si>
-    <t>intermediate 1</t>
-  </si>
-  <si>
     <t>wire2</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>_201107</t>
   </si>
   <si>
-    <t>_201108</t>
-  </si>
-  <si>
     <t>cable1</t>
   </si>
   <si>
@@ -520,6 +511,36 @@
   </si>
   <si>
     <t>_311046-2</t>
+  </si>
+  <si>
+    <t>wire3</t>
+  </si>
+  <si>
+    <t>_201204</t>
+  </si>
+  <si>
+    <t>_201206</t>
+  </si>
+  <si>
+    <t>_201207</t>
+  </si>
+  <si>
+    <t>_311050-1</t>
+  </si>
+  <si>
+    <t>_311050-2</t>
+  </si>
+  <si>
+    <t>_311051-2</t>
+  </si>
+  <si>
+    <t>_311051-1 connected join to _311050</t>
+  </si>
+  <si>
+    <t>_311052-1</t>
+  </si>
+  <si>
+    <t>_311052-2</t>
   </si>
 </sst>
 </file>
@@ -857,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -879,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,40 +913,43 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="E6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -933,728 +957,751 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" t="s">
-        <v>155</v>
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
-        <v>157</v>
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" t="s">
-        <v>136</v>
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
         <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
         <v>56</v>
       </c>
-      <c r="D32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" t="s">
-        <v>66</v>
-      </c>
-      <c r="E40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>86</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D46" t="s">
         <v>68</v>
       </c>
-      <c r="E42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+      <c r="E46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>87</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D47" t="s">
         <v>69</v>
       </c>
-      <c r="E43" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="E47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>88</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D48" t="s">
         <v>70</v>
       </c>
-      <c r="E44" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" t="s">
-        <v>71</v>
-      </c>
-      <c r="E45" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>90</v>
-      </c>
-      <c r="D46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" t="s">
-        <v>74</v>
-      </c>
       <c r="E48" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D49" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E49" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D50" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E50" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E51" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D53" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E53" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D54" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E54" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" t="s">
-        <v>100</v>
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" t="s">
-        <v>109</v>
-      </c>
-      <c r="E60" t="s">
-        <v>136</v>
+      <c r="A60" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D61" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E61" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E62" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D63" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E63" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>113</v>
-      </c>
-      <c r="B64" t="s">
-        <v>114</v>
+      <c r="C64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D64" t="s">
+        <v>109</v>
+      </c>
+      <c r="E64" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>52</v>
-      </c>
-      <c r="D65" t="s">
-        <v>115</v>
-      </c>
-      <c r="E65" t="s">
-        <v>136</v>
+      <c r="A65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D66" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E66" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D67" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E67" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D68" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E68" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" t="s">
-        <v>120</v>
+      <c r="C69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D69" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>127</v>
-      </c>
-      <c r="D70" t="s">
-        <v>121</v>
-      </c>
-      <c r="E70" t="s">
-        <v>136</v>
+      <c r="A70" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D71" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E71" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" t="s">
-        <v>124</v>
+      <c r="C72" t="s">
+        <v>125</v>
+      </c>
+      <c r="D72" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" t="s">
-        <v>125</v>
-      </c>
-      <c r="E73" t="s">
-        <v>136</v>
+      <c r="A73" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D74" t="s">
+        <v>122</v>
+      </c>
+      <c r="E74" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>125</v>
+      </c>
+      <c r="D75" t="s">
+        <v>123</v>
+      </c>
+      <c r="E75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>126</v>
       </c>
-      <c r="E74" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>129</v>
-      </c>
-      <c r="B75" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
+      <c r="B76" t="s">
         <v>127</v>
-      </c>
-      <c r="D76" t="s">
-        <v>131</v>
-      </c>
-      <c r="E76" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
+        <v>124</v>
+      </c>
+      <c r="D77" t="s">
         <v>128</v>
       </c>
-      <c r="D77" t="s">
-        <v>132</v>
-      </c>
       <c r="E77" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>133</v>
-      </c>
-      <c r="B78" t="s">
-        <v>134</v>
+      <c r="C78" t="s">
+        <v>125</v>
+      </c>
+      <c r="D78" t="s">
+        <v>129</v>
+      </c>
+      <c r="E78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>130</v>
+      </c>
+      <c r="B79" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>